<commit_message>
update package, unit tests and validation
</commit_message>
<xml_diff>
--- a/tdcrpy/validation/Validation_Interaction.xlsx
+++ b/tdcrpy/validation/Validation_Interaction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python_modules\TDCRPy\TDCRPy\tdcrpy\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC03C94F-0F42-4FFE-B829-315FB9215CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A159D3-1A97-46D7-B01A-663628C9B330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3555" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t xml:space="preserve">validation of the function energie_dep_gamma2() </t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>N trials</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>u(E) /keV</t>
+  </si>
+  <si>
+    <t>V /ml</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>E incidente</a:t>
+                  <a:t>Volume /ml</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1343,7 +1343,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9FB7843-80C0-41F5-B9A9-78622C05B7CA}" name="Table1" displayName="Table1" ref="A8:C21" totalsRowShown="0">
   <autoFilter ref="A8:C21" xr:uid="{F9FB7843-80C0-41F5-B9A9-78622C05B7CA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{65E01827-C436-4ED3-A6FA-4C1DBA4CD9DF}" name="V"/>
+    <tableColumn id="1" xr3:uid="{65E01827-C436-4ED3-A6FA-4C1DBA4CD9DF}" name="V /ml"/>
     <tableColumn id="2" xr3:uid="{B2CE250D-A68B-4A4C-8F7A-FE0DE53D1340}" name="E /keV"/>
     <tableColumn id="3" xr3:uid="{78E35C38-2D95-4F50-86F9-7E85A05A1E09}" name="u(E) /keV"/>
   </tableColumns>
@@ -1617,48 +1617,48 @@
   <dimension ref="A5:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>10000</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>15</v>
       </c>
       <c r="F7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
profiling - develop interpolated quenching energies
</commit_message>
<xml_diff>
--- a/tdcrpy/validation/Validation_Interaction.xlsx
+++ b/tdcrpy/validation/Validation_Interaction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python_modules\TDCRPy\TDCRPy\tdcrpy\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A159D3-1A97-46D7-B01A-663628C9B330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC3E607-D17B-4012-A7D3-672EDA6205ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,10 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1617,7 +1625,7 @@
   <dimension ref="A5:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1681,13 +1689,13 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="4">
         <v>7.1</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -1747,13 +1755,13 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>7.76</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start quadratic function for the interaction
</commit_message>
<xml_diff>
--- a/tdcrpy/validation/Validation_Interaction.xlsx
+++ b/tdcrpy/validation/Validation_Interaction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python_modules\TDCRPy\TDCRPy\tdcrpy\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC3E607-D17B-4012-A7D3-672EDA6205ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA0E256-266F-4AAD-B63A-D00A37C90243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t xml:space="preserve">validation of the function energie_dep_gamma2() </t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>V /ml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation of the function energie_dep_beta2() </t>
   </si>
 </sst>
 </file>
@@ -69,18 +72,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,12 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -211,96 +205,730 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$9:$C$21</c:f>
+                <c:f>Sheet1!$C$9:$C$29</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="13"/>
+                  <c:ptCount val="21"/>
                   <c:pt idx="0">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4557957312670495E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4617002688326106E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4694884723376195E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4686597163499194E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4697921538955797E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4778102687885095E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4752420558667695E-2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4790511063559106E-2</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4737929765358105E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4625633007698297E-2</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4653477011864505E-2</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4600154356024101E-2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>7.4443674320063297E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$9:$C$21</c:f>
+                <c:f>Sheet1!$C$9:$C$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="21"/>
+                  <c:pt idx="0">
+                    <c:v>7.4557957312670495E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.4617002688326106E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.4694884723376195E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.4686597163499194E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.4697921538955797E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.4778102687885095E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.4752420558667695E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.4790511063559106E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.4737929765358105E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>7.4625633007698297E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.4653477011864505E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.4600154356024101E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>7.4443674320063297E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$9:$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>validation of the function energie_dep_beta2() </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>6.9610817799999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0144972999999897</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.16771229999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1419451199999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1767301999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4732281599999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5995557199999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6096299399999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6821999799999903</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.8991198799999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.9221921200000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0063688600000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1876379400000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DAD3-4266-87FC-9D6F12C2E238}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1137214175"/>
+        <c:axId val="1137205055"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1137214175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Volume /ml</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137205055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1137205055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>E déposée /keV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137214175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E /keV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$32:$C$44</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="13"/>
                   <c:pt idx="0">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.8640315089152697</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.8893061577955397</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.7665763753735204</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.6903443198632502</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.7150197197733297</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.6379407739051199</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.6676500476096097</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.5975781973472003</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.5685409393618297</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.48546976227136</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.5290597854344803</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.4306149110481696</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>4.3630310760600404</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$32:$C$44</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>4.8640315089152697</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.8893061577955397</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.7665763753735204</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.6903443198632502</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.7150197197733297</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.6379407739051199</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.6676500476096097</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5975781973472003</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.5685409393618297</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.48546976227136</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4.5290597854344803</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.4306149110481696</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>4.3630310760600404</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -321,7 +949,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$9:$A$21</c:f>
+              <c:f>Sheet1!$A$32:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -369,48 +997,48 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$21</c:f>
+              <c:f>Sheet1!$B$32:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>7.04</c:v>
+                  <c:v>1173.1713883</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.99</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.00">
-                  <c:v>7.1</c:v>
+                  <c:v>1167.6768858999901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1192.5617689000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.18</c:v>
+                  <c:v>1201.3945151999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.24</c:v>
+                  <c:v>1201.5473526999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.32</c:v>
+                  <c:v>1211.54486059999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.44</c:v>
+                  <c:v>1207.7114609</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.59</c:v>
+                  <c:v>1226.9916456000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.76</c:v>
+                  <c:v>1225.9456232999901</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.71</c:v>
+                  <c:v>1240.5849143999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.87</c:v>
+                  <c:v>1235.3133806000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.06</c:v>
+                  <c:v>1246.72590729999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.19</c:v>
+                  <c:v>1257.0787886999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,7 +1046,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DAD3-4266-87FC-9D6F12C2E238}"/>
+              <c16:uniqueId val="{00000000-5BB1-4119-90F6-BFD0F0FC343A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -790,7 +1418,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1344,6 +2528,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4B0AAAF-CD56-4AAB-850F-F1E4D932E0B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1354,6 +2576,18 @@
     <tableColumn id="1" xr3:uid="{65E01827-C436-4ED3-A6FA-4C1DBA4CD9DF}" name="V /ml"/>
     <tableColumn id="2" xr3:uid="{B2CE250D-A68B-4A4C-8F7A-FE0DE53D1340}" name="E /keV"/>
     <tableColumn id="3" xr3:uid="{78E35C38-2D95-4F50-86F9-7E85A05A1E09}" name="u(E) /keV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79EEFB42-B463-4BCF-82C6-2374849217C2}" name="Table13" displayName="Table13" ref="A31:C44" totalsRowShown="0">
+  <autoFilter ref="A31:C44" xr:uid="{79EEFB42-B463-4BCF-82C6-2374849217C2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{18953E56-195E-4AE8-BD90-2C525BF57C8A}" name="V /ml"/>
+    <tableColumn id="2" xr3:uid="{54E85AEF-C773-431D-B5EB-E2B74FBB87B8}" name="E /keV"/>
+    <tableColumn id="3" xr3:uid="{EF0E0C62-5A32-4A24-9F9A-03250BA24A7F}" name="u(E) /keV"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1622,23 +2856,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:F21"/>
+  <dimension ref="A5:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1655,7 +2889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1666,155 +2900,535 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>7.04</v>
+        <v>6.9610817799999998</v>
       </c>
       <c r="C9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.4557957312670495E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>6.99</v>
+        <v>7.0144972999999897</v>
       </c>
       <c r="C10">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+        <v>7.4617002688326106E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
-        <v>7.1</v>
-      </c>
-      <c r="C11" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>7.16771229999999</v>
+      </c>
+      <c r="C11">
+        <v>7.4694884723376195E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>7.18</v>
+        <v>7.1419451199999999</v>
       </c>
       <c r="C12">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.4686597163499194E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>7.24</v>
-      </c>
-      <c r="C13" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.1767301999999997</v>
+      </c>
+      <c r="C13">
+        <v>7.4697921538955797E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>7.32</v>
+        <v>7.4732281599999997</v>
       </c>
       <c r="C14">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.4778102687885095E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>7.44</v>
-      </c>
-      <c r="C15" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.5995557199999997</v>
+      </c>
+      <c r="C15">
+        <v>7.4752420558667695E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>7.59</v>
+        <v>7.6096299399999996</v>
       </c>
       <c r="C16">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+        <v>7.4790511063559106E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>7.76</v>
-      </c>
-      <c r="C17" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>7.6821999799999903</v>
+      </c>
+      <c r="C17">
+        <v>7.4737929765358105E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>7.71</v>
+        <v>7.8991198799999998</v>
       </c>
       <c r="C18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7.4625633007698297E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>7.87</v>
+        <v>7.9221921200000001</v>
       </c>
       <c r="C19">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7.4653477011864505E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.06</v>
+        <v>8.0063688600000003</v>
       </c>
       <c r="C20">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7.4600154356024101E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>8.19</v>
+        <v>8.1876379400000001</v>
       </c>
       <c r="C21">
-        <v>7.0000000000000007E-2</v>
+        <v>7.4443674320063297E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>10000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>1500</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>1118.73774449999</v>
+      </c>
+      <c r="T31">
+        <v>5.0744873649891904</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>1173.1713883</v>
+      </c>
+      <c r="C32">
+        <v>4.8640315089152697</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1121.12595159999</v>
+      </c>
+      <c r="T32">
+        <v>5.0557357438877704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>1167.6768858999901</v>
+      </c>
+      <c r="C33">
+        <v>4.8893061577955397</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>1132.2439503999999</v>
+      </c>
+      <c r="T33">
+        <v>5.0285307069710603</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>1192.5617689000001</v>
+      </c>
+      <c r="C34">
+        <v>4.7665763753735204</v>
+      </c>
+      <c r="R34">
+        <v>3</v>
+      </c>
+      <c r="S34">
+        <v>1144.58214169999</v>
+      </c>
+      <c r="T34">
+        <v>4.98549233413216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>1201.3945151999999</v>
+      </c>
+      <c r="C35">
+        <v>4.6903443198632502</v>
+      </c>
+      <c r="R35">
+        <v>4</v>
+      </c>
+      <c r="S35">
+        <v>1148.6559431000001</v>
+      </c>
+      <c r="T35">
+        <v>4.9554420860744104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>1201.5473526999999</v>
+      </c>
+      <c r="C36">
+        <v>4.7150197197733297</v>
+      </c>
+      <c r="R36">
+        <v>5</v>
+      </c>
+      <c r="S36">
+        <v>1151.6292277999901</v>
+      </c>
+      <c r="T36">
+        <v>4.9293196932576002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>1211.54486059999</v>
+      </c>
+      <c r="C37">
+        <v>4.6379407739051199</v>
+      </c>
+      <c r="R37">
+        <v>6</v>
+      </c>
+      <c r="S37">
+        <v>1160.9782855000001</v>
+      </c>
+      <c r="T37">
+        <v>4.9256184868217696</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>1207.7114609</v>
+      </c>
+      <c r="C38">
+        <v>4.6676500476096097</v>
+      </c>
+      <c r="R38">
+        <v>7</v>
+      </c>
+      <c r="S38">
+        <v>1163.7738711</v>
+      </c>
+      <c r="T38">
+        <v>4.8952311458320299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>1226.9916456000001</v>
+      </c>
+      <c r="C39">
+        <v>4.5975781973472003</v>
+      </c>
+      <c r="R39">
+        <v>8</v>
+      </c>
+      <c r="S39">
+        <v>1173.1713883</v>
+      </c>
+      <c r="T39">
+        <v>4.8640315089152697</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>1225.9456232999901</v>
+      </c>
+      <c r="C40">
+        <v>4.5685409393618297</v>
+      </c>
+      <c r="R40">
+        <v>9</v>
+      </c>
+      <c r="S40">
+        <v>1167.6768858999901</v>
+      </c>
+      <c r="T40">
+        <v>4.8893061577955397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>1240.5849143999999</v>
+      </c>
+      <c r="C41">
+        <v>4.48546976227136</v>
+      </c>
+      <c r="R41">
+        <v>10</v>
+      </c>
+      <c r="S41">
+        <v>1192.5617689000001</v>
+      </c>
+      <c r="T41">
+        <v>4.7665763753735204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18</v>
+      </c>
+      <c r="B42">
+        <v>1235.3133806000001</v>
+      </c>
+      <c r="C42">
+        <v>4.5290597854344803</v>
+      </c>
+      <c r="R42">
+        <v>11</v>
+      </c>
+      <c r="S42">
+        <v>1201.3945151999999</v>
+      </c>
+      <c r="T42">
+        <v>4.6903443198632502</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <v>1246.72590729999</v>
+      </c>
+      <c r="C43">
+        <v>4.4306149110481696</v>
+      </c>
+      <c r="R43">
+        <v>12</v>
+      </c>
+      <c r="S43">
+        <v>1201.5473526999999</v>
+      </c>
+      <c r="T43">
+        <v>4.7150197197733297</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>1257.0787886999999</v>
+      </c>
+      <c r="C44">
+        <v>4.3630310760600404</v>
+      </c>
+      <c r="R44">
+        <v>13</v>
+      </c>
+      <c r="S44">
+        <v>1211.54486059999</v>
+      </c>
+      <c r="T44">
+        <v>4.6379407739051199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>14</v>
+      </c>
+      <c r="S45">
+        <v>1207.7114609</v>
+      </c>
+      <c r="T45">
+        <v>4.6676500476096097</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>15</v>
+      </c>
+      <c r="S46">
+        <v>1226.9916456000001</v>
+      </c>
+      <c r="T46">
+        <v>4.5975781973472003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>16</v>
+      </c>
+      <c r="S47">
+        <v>1225.9456232999901</v>
+      </c>
+      <c r="T47">
+        <v>4.5685409393618297</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>17</v>
+      </c>
+      <c r="S48">
+        <v>1240.5849143999999</v>
+      </c>
+      <c r="T48">
+        <v>4.48546976227136</v>
+      </c>
+    </row>
+    <row r="49" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>18</v>
+      </c>
+      <c r="S49">
+        <v>1235.3133806000001</v>
+      </c>
+      <c r="T49">
+        <v>4.5290597854344803</v>
+      </c>
+    </row>
+    <row r="50" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>19</v>
+      </c>
+      <c r="S50">
+        <v>1246.72590729999</v>
+      </c>
+      <c r="T50">
+        <v>4.4306149110481696</v>
+      </c>
+    </row>
+    <row r="51" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R51">
+        <v>20</v>
+      </c>
+      <c r="S51">
+        <v>1257.0787886999999</v>
+      </c>
+      <c r="T51">
+        <v>4.3630310760600404</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test volume with quadratic fct
</commit_message>
<xml_diff>
--- a/tdcrpy/validation/Validation_Interaction.xlsx
+++ b/tdcrpy/validation/Validation_Interaction.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python_modules\TDCRPy\TDCRPy\tdcrpy\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA0E256-266F-4AAD-B63A-D00A37C90243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9D437A-6AEF-4589-8139-A968A4A38B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t xml:space="preserve">validation of the function energie_dep_gamma2() </t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">validation of the function energie_dep_beta2() </t>
+  </si>
+  <si>
+    <t>v linear</t>
+  </si>
+  <si>
+    <t>v quadratic</t>
   </si>
 </sst>
 </file>
@@ -126,36 +133,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -166,15 +143,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>E /keV</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>lineaire</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -205,96 +174,96 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$9:$C$29</c:f>
+                <c:f>'Sheet1 (2)'!$C$9:$C$29</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="21"/>
                   <c:pt idx="0">
-                    <c:v>7.4557957312670495E-2</c:v>
+                    <c:v>2.35669202107146E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.4617002688326106E-2</c:v>
+                    <c:v>2.3587033860985901E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.4694884723376195E-2</c:v>
+                    <c:v>2.3606751926462399E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4686597163499194E-2</c:v>
+                    <c:v>2.36226804354344E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.4697921538955797E-2</c:v>
+                    <c:v>2.3634691875766198E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.4778102687885095E-2</c:v>
+                    <c:v>2.3638401009090201E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>7.4752420558667695E-2</c:v>
+                    <c:v>2.3642286011787701E-2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7.4790511063559106E-2</c:v>
+                    <c:v>2.3638524668528001E-2</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.4737929765358105E-2</c:v>
+                    <c:v>2.3635674938519001E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>7.4625633007698297E-2</c:v>
+                    <c:v>2.36207099954957E-2</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>7.4653477011864505E-2</c:v>
+                    <c:v>2.3608125202996301E-2</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>7.4600154356024101E-2</c:v>
+                    <c:v>2.35860547360035E-2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>7.4443674320063297E-2</c:v>
+                    <c:v>2.3566766457542101E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$9:$C$29</c:f>
+                <c:f>'Sheet1 (2)'!$C$9:$C$29</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="21"/>
                   <c:pt idx="0">
-                    <c:v>7.4557957312670495E-2</c:v>
+                    <c:v>2.35669202107146E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.4617002688326106E-2</c:v>
+                    <c:v>2.3587033860985901E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.4694884723376195E-2</c:v>
+                    <c:v>2.3606751926462399E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4686597163499194E-2</c:v>
+                    <c:v>2.36226804354344E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>7.4697921538955797E-2</c:v>
+                    <c:v>2.3634691875766198E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>7.4778102687885095E-2</c:v>
+                    <c:v>2.3638401009090201E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>7.4752420558667695E-2</c:v>
+                    <c:v>2.3642286011787701E-2</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7.4790511063559106E-2</c:v>
+                    <c:v>2.3638524668528001E-2</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.4737929765358105E-2</c:v>
+                    <c:v>2.3635674938519001E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>7.4625633007698297E-2</c:v>
+                    <c:v>2.36207099954957E-2</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>7.4653477011864505E-2</c:v>
+                    <c:v>2.3608125202996301E-2</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>7.4600154356024101E-2</c:v>
+                    <c:v>2.35860547360035E-2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>7.4443674320063297E-2</c:v>
+                    <c:v>2.3566766457542101E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -314,10 +283,11 @@
             </c:spPr>
           </c:errBars>
           <c:xVal>
-            <c:strRef>
-              <c:f>Sheet1!$A$9:$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="19"/>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$9:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
@@ -357,56 +327,53 @@
                 <c:pt idx="12">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>validation of the function energie_dep_beta2() </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$B$29</c:f>
+              <c:f>'Sheet1 (2)'!$B$9:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>6.9610817799999998</c:v>
+                  <c:v>6.9126306199999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.0144972999999897</c:v>
+                  <c:v>7.0072507259999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.16771229999999</c:v>
+                  <c:v>7.0994776479999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1419451199999999</c:v>
+                  <c:v>7.2073613639999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1767301999999997</c:v>
+                  <c:v>7.2977762879999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.4732281599999997</c:v>
+                  <c:v>7.5073114299999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.5995557199999997</c:v>
+                  <c:v>7.5212081900000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.6096299399999996</c:v>
+                  <c:v>7.6362715899999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.6821999799999903</c:v>
+                  <c:v>7.67758071</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.8991198799999998</c:v>
+                  <c:v>7.8351304079999897</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9221921200000001</c:v>
+                  <c:v>7.9032242420000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.0063688600000003</c:v>
+                  <c:v>8.0147961520000006</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.1876379400000001</c:v>
+                  <c:v>8.1106760799999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,7 +381,253 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DAD3-4266-87FC-9D6F12C2E238}"/>
+              <c16:uniqueId val="{00000000-8D2E-4117-9DEC-461480A8FAC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>quadratic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$I$9:$I$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>7.8340709696572905E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3304786834530006E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.1548465066776904E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3155555908589293E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.6425912765541305E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.3826061493181003E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.7748179068160195E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.8626998765953396E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>8.8344876228231506E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.6070089887129303E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>8.8813662248044198E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.9820984558401401E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>8.9213050792305307E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$I$9:$I$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>7.8340709696572905E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3304786834530006E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.1548465066776904E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.3155555908589293E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.6425912765541305E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.3826061493181003E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.7748179068160195E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.8626998765953396E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>8.8344876228231506E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.6070089887129303E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>8.8813662248044198E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>8.9820984558401401E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>8.9213050792305307E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$G$9:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$H$9:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>2.34090358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5543152</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5881083999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5175684600000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.80318522</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.75663766</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8421203199999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9446477999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0318970799999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8021405800000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9545055800000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0114751399999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.03123136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8D2E-4117-9DEC-461480A8FAC2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -747,6 +960,1479 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E /keV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$C$32:$C$44</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>4.8640315089152697</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.8893061577955397</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.7665763753735204</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.6903443198632502</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.7150197197733297</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.6379407739051199</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.6676500476096097</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5975781973472003</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.5685409393618297</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.48546976227136</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4.5290597854344803</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.4306149110481696</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>4.3630310760600404</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Sheet1 (2)'!$C$32:$C$44</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>4.8640315089152697</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.8893061577955397</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.7665763753735204</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4.6903443198632502</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.7150197197733297</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.6379407739051199</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.6676500476096097</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>4.5975781973472003</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.5685409393618297</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4.48546976227136</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4.5290597854344803</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.4306149110481696</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>4.3630310760600404</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$32:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$32:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1173.1713883</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1167.6768858999901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1192.5617689000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1201.3945151999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1201.5473526999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1211.54486059999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1207.7114609</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1226.9916456000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1225.9456232999901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1240.5849143999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1235.3133806000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1246.72590729999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1257.0787886999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B88-4BA7-B590-AAB145CAB531}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1137214175"/>
+        <c:axId val="1137205055"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1137214175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Volume /ml</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137205055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1137205055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>E déposée /keV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137214175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>lineaire</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$9:$C$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="21"/>
+                  <c:pt idx="0">
+                    <c:v>2.35669202107146E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.3587033860985901E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.3606751926462399E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.36226804354344E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.3634691875766198E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.3638401009090201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.3642286011787701E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.3638524668528001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.3635674938519001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.36207099954957E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.3608125202996301E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.35860547360035E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.3566766457542101E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$9:$C$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="21"/>
+                  <c:pt idx="0">
+                    <c:v>2.35669202107146E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.3587033860985901E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.3606751926462399E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.36226804354344E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.3634691875766198E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.3638401009090201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.3642286011787701E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.3638524668528001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.3635674938519001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.36207099954957E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.3608125202996301E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.35860547360035E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.3566766457542101E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$9:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.9126306199999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0072507259999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0994776479999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2073613639999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2977762879999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5073114299999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5212081900000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6362715899999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.67758071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.8351304079999897</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.9032242420000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0147961520000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1106760799999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DAD3-4266-87FC-9D6F12C2E238}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>quadratic</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$I$9:$I$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>2.35179363950868E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.3569068632171598E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.3605186587696201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.36301116679953E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.3637814937406201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.3641142036443501E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.3639375029396701E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.3637043705172701E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.36300157502379E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.3621782838380199E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.3630905011029199E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.3633705121885399E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.36327789001173E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$I$9:$I$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="13"/>
+                  <c:pt idx="0">
+                    <c:v>2.35179363950868E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.3569068632171598E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.3605186587696201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.36301116679953E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.3637814937406201E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.3641142036443501E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.3639375029396701E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.3637043705172701E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.36300157502379E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2.3621782838380199E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.3630905011029199E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.3633705121885399E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.36327789001173E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$9:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$9:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.7345806140000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9155103759999896</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0913810359999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.2491888580000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3665055659999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4802146179999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5633341819999904</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6477981519999902</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.7358897139999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.789710328</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.73432420199999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.7038543519999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.7237069680000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9BC5-4852-94A9-602E79EDB7F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1137214175"/>
+        <c:axId val="1137205055"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1137214175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Volume /ml</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137205055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1137205055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="6"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>E déposée /keV</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1137214175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1458,6 +3144,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2490,20 +4256,1133 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F8A547E-DDB8-4B61-BCBA-2A0AC529CE66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7855D802-4298-4475-BFCE-6ED81E089B20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2570,6 +5449,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9425BF1F-FA6E-4352-8A55-48F509B4302D}" name="Table15" displayName="Table15" ref="A8:C21" totalsRowShown="0">
+  <autoFilter ref="A8:C21" xr:uid="{F9FB7843-80C0-41F5-B9A9-78622C05B7CA}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3E72D530-BAC6-4DDD-B55C-D36E1D2F57F8}" name="V /ml"/>
+    <tableColumn id="2" xr3:uid="{B0C47E0B-0677-4173-AFD2-F4005B3D9F93}" name="E /keV"/>
+    <tableColumn id="3" xr3:uid="{6AF9598D-FD9C-428A-92E6-B99DF4EDAFCD}" name="u(E) /keV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{ED8EC204-979D-4E2D-B9C0-9E03B60E8AA9}" name="Table136" displayName="Table136" ref="A31:C44" totalsRowShown="0">
+  <autoFilter ref="A31:C44" xr:uid="{79EEFB42-B463-4BCF-82C6-2374849217C2}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{96271534-6881-433E-907B-011A5D804FC1}" name="V /ml"/>
+    <tableColumn id="2" xr3:uid="{76CA59A0-216C-44C3-B0C8-3F8C199BFDEC}" name="E /keV"/>
+    <tableColumn id="3" xr3:uid="{AD89E15C-FD78-4380-8EB0-04D04032AC72}" name="u(E) /keV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{28E34AD9-1837-461F-815A-A3D8795BF0E2}" name="Table147" displayName="Table147" ref="G8:I21" totalsRowShown="0">
+  <autoFilter ref="G8:I21" xr:uid="{99EC42C4-B6B9-41B8-88C0-D3B478E0606B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5C332655-C458-4A06-A174-1F0DEC62D4CA}" name="V /ml"/>
+    <tableColumn id="2" xr3:uid="{228D8D98-8F45-4204-B2FA-8CB1CF7F8E91}" name="E /keV"/>
+    <tableColumn id="3" xr3:uid="{CAE617DB-DCF5-457D-A832-BFEBF101F45A}" name="u(E) /keV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9FB7843-80C0-41F5-B9A9-78622C05B7CA}" name="Table1" displayName="Table1" ref="A8:C21" totalsRowShown="0">
   <autoFilter ref="A8:C21" xr:uid="{F9FB7843-80C0-41F5-B9A9-78622C05B7CA}"/>
   <tableColumns count="3">
@@ -2581,13 +5496,25 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79EEFB42-B463-4BCF-82C6-2374849217C2}" name="Table13" displayName="Table13" ref="A31:C44" totalsRowShown="0">
   <autoFilter ref="A31:C44" xr:uid="{79EEFB42-B463-4BCF-82C6-2374849217C2}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{18953E56-195E-4AE8-BD90-2C525BF57C8A}" name="V /ml"/>
     <tableColumn id="2" xr3:uid="{54E85AEF-C773-431D-B5EB-E2B74FBB87B8}" name="E /keV"/>
     <tableColumn id="3" xr3:uid="{EF0E0C62-5A32-4A24-9F9A-03250BA24A7F}" name="u(E) /keV"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{99EC42C4-B6B9-41B8-88C0-D3B478E0606B}" name="Table14" displayName="Table14" ref="G8:I21" totalsRowShown="0">
+  <autoFilter ref="G8:I21" xr:uid="{99EC42C4-B6B9-41B8-88C0-D3B478E0606B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B0E38161-BEEB-41C6-9689-961F900E5AF8}" name="V /ml"/>
+    <tableColumn id="2" xr3:uid="{4C88277F-EB88-4B76-BC82-665953DB625B}" name="E /keV"/>
+    <tableColumn id="3" xr3:uid="{3C80B2AE-26F4-4057-B007-FF44A789B0D4}" name="u(E) /keV"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2855,11 +5782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15F4CB94-1329-4C41-A132-B90AEBD542A9}">
   <dimension ref="A5:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="G9" sqref="G9:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2867,12 +5794,20 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2889,7 +5824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2899,93 +5834,246 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>6.9610817799999998</v>
+        <v>6.9126306199999998</v>
       </c>
       <c r="C9">
-        <v>7.4557957312670495E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.35669202107146E-2</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>2.34090358</v>
+      </c>
+      <c r="I9">
+        <v>7.8340709696572905E-2</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>2.34090358</v>
+      </c>
+      <c r="M9">
+        <v>7.8340709696572905E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>7.0144972999999897</v>
+        <v>7.0072507259999997</v>
       </c>
       <c r="C10">
-        <v>7.4617002688326106E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.3587033860985901E-2</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>2.5543152</v>
+      </c>
+      <c r="I10">
+        <v>8.3304786834530006E-2</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>2.5543152</v>
+      </c>
+      <c r="M10">
+        <v>8.3304786834530006E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>7.16771229999999</v>
+        <v>7.0994776479999997</v>
       </c>
       <c r="C11">
-        <v>7.4694884723376195E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.3606751926462399E-2</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>2.5881083999999999</v>
+      </c>
+      <c r="I11">
+        <v>8.1548465066776904E-2</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>2.5881083999999999</v>
+      </c>
+      <c r="M11">
+        <v>8.1548465066776904E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>7.1419451199999999</v>
+        <v>7.2073613639999996</v>
       </c>
       <c r="C12">
-        <v>7.4686597163499194E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.36226804354344E-2</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>2.5175684600000001</v>
+      </c>
+      <c r="I12">
+        <v>8.3155555908589293E-2</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>2.5175684600000001</v>
+      </c>
+      <c r="M12">
+        <v>8.3155555908589293E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>7.1767301999999997</v>
+        <v>7.2977762879999997</v>
       </c>
       <c r="C13">
-        <v>7.4697921538955797E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.3634691875766198E-2</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>2.80318522</v>
+      </c>
+      <c r="I13">
+        <v>8.6425912765541305E-2</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>2.80318522</v>
+      </c>
+      <c r="M13">
+        <v>8.6425912765541305E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>7.4732281599999997</v>
+        <v>7.5073114299999997</v>
       </c>
       <c r="C14">
-        <v>7.4778102687885095E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.3638401009090201E-2</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>2.75663766</v>
+      </c>
+      <c r="I14">
+        <v>8.3826061493181003E-2</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>2.75663766</v>
+      </c>
+      <c r="M14">
+        <v>8.3826061493181003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>7.5995557199999997</v>
+        <v>7.5212081900000003</v>
       </c>
       <c r="C15">
-        <v>7.4752420558667695E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2.3642286011787701E-2</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>2.8421203199999998</v>
+      </c>
+      <c r="I15">
+        <v>8.7748179068160195E-2</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>2.8421203199999998</v>
+      </c>
+      <c r="M15">
+        <v>8.7748179068160195E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>7.6096299399999996</v>
+        <v>7.6362715899999998</v>
       </c>
       <c r="C16">
-        <v>7.4790511063559106E-2</v>
+        <v>2.3638524668528001E-2</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>2.9446477999999998</v>
+      </c>
+      <c r="I16">
+        <v>8.8626998765953396E-2</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>2.9446477999999998</v>
+      </c>
+      <c r="M16">
+        <v>8.8626998765953396E-2</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -2993,10 +6081,28 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>7.6821999799999903</v>
+        <v>7.67758071</v>
       </c>
       <c r="C17">
-        <v>7.4737929765358105E-2</v>
+        <v>2.3635674938519001E-2</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>3.0318970799999998</v>
+      </c>
+      <c r="I17">
+        <v>8.8344876228231506E-2</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>3.0318970799999998</v>
+      </c>
+      <c r="M17">
+        <v>8.8344876228231506E-2</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
@@ -3004,10 +6110,28 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>7.8991198799999998</v>
+        <v>7.8351304079999897</v>
       </c>
       <c r="C18">
-        <v>7.4625633007698297E-2</v>
+        <v>2.36207099954957E-2</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>2.8021405800000001</v>
+      </c>
+      <c r="I18">
+        <v>8.6070089887129303E-2</v>
+      </c>
+      <c r="K18">
+        <v>17</v>
+      </c>
+      <c r="L18">
+        <v>2.8021405800000001</v>
+      </c>
+      <c r="M18">
+        <v>8.6070089887129303E-2</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
@@ -3015,10 +6139,28 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>7.9221921200000001</v>
+        <v>7.9032242420000003</v>
       </c>
       <c r="C19">
-        <v>7.4653477011864505E-2</v>
+        <v>2.3608125202996301E-2</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>2.9545055800000002</v>
+      </c>
+      <c r="I19">
+        <v>8.8813662248044198E-2</v>
+      </c>
+      <c r="K19">
+        <v>18</v>
+      </c>
+      <c r="L19">
+        <v>2.9545055800000002</v>
+      </c>
+      <c r="M19">
+        <v>8.8813662248044198E-2</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -3026,10 +6168,28 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>8.0063688600000003</v>
+        <v>8.0147961520000006</v>
       </c>
       <c r="C20">
-        <v>7.4600154356024101E-2</v>
+        <v>2.35860547360035E-2</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>3.0114751399999999</v>
+      </c>
+      <c r="I20">
+        <v>8.9820984558401401E-2</v>
+      </c>
+      <c r="K20">
+        <v>19</v>
+      </c>
+      <c r="L20">
+        <v>3.0114751399999999</v>
+      </c>
+      <c r="M20">
+        <v>8.9820984558401401E-2</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -3037,10 +6197,28 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>8.1876379400000001</v>
+        <v>8.1106760799999993</v>
       </c>
       <c r="C21">
-        <v>7.4443674320063297E-2</v>
+        <v>2.3566766457542101E-2</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>3.03123136</v>
+      </c>
+      <c r="I21">
+        <v>8.9213050792305307E-2</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="L21">
+        <v>3.03123136</v>
+      </c>
+      <c r="M21">
+        <v>8.9213050792305307E-2</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
@@ -3426,9 +6604,841 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A5:T51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>10000</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>6.9126306199999998</v>
+      </c>
+      <c r="C9">
+        <v>2.35669202107146E-2</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>6.7345806140000004</v>
+      </c>
+      <c r="I9">
+        <v>2.35179363950868E-2</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>5.4176057200000001</v>
+      </c>
+      <c r="M9">
+        <v>0.18285275648922</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>7.0072507259999997</v>
+      </c>
+      <c r="C10">
+        <v>2.3587033860985901E-2</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>6.9155103759999896</v>
+      </c>
+      <c r="I10">
+        <v>2.3569068632171598E-2</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>5.5527432799999996</v>
+      </c>
+      <c r="M10">
+        <v>0.18230384125879401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>7.0994776479999997</v>
+      </c>
+      <c r="C11">
+        <v>2.3606751926462399E-2</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>7.0913810359999996</v>
+      </c>
+      <c r="I11">
+        <v>2.3605186587696201E-2</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>5.8592807199999903</v>
+      </c>
+      <c r="M11">
+        <v>0.18899116517558201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>7.2073613639999996</v>
+      </c>
+      <c r="C12">
+        <v>2.36226804354344E-2</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>7.2491888580000001</v>
+      </c>
+      <c r="I12">
+        <v>2.36301116679953E-2</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>5.9688995</v>
+      </c>
+      <c r="M12">
+        <v>0.19333451178232999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7.2977762879999997</v>
+      </c>
+      <c r="C13">
+        <v>2.3634691875766198E-2</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>7.3665055659999998</v>
+      </c>
+      <c r="I13">
+        <v>2.3637814937406201E-2</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>6.3061426000000003</v>
+      </c>
+      <c r="M13">
+        <v>0.20101775490714399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>7.5073114299999997</v>
+      </c>
+      <c r="C14">
+        <v>2.3638401009090201E-2</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>7.4802146179999998</v>
+      </c>
+      <c r="I14">
+        <v>2.3641142036443501E-2</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>6.3530906799999904</v>
+      </c>
+      <c r="M14">
+        <v>0.195987713347552</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>7.5212081900000003</v>
+      </c>
+      <c r="C15">
+        <v>2.3642286011787701E-2</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>7.5633341819999904</v>
+      </c>
+      <c r="I15">
+        <v>2.3639375029396701E-2</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>6.5231460999999999</v>
+      </c>
+      <c r="M15">
+        <v>0.202676326554633</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>7.6362715899999998</v>
+      </c>
+      <c r="C16">
+        <v>2.3638524668528001E-2</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>7.6477981519999902</v>
+      </c>
+      <c r="I16">
+        <v>2.3637043705172701E-2</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>6.5969392600000001</v>
+      </c>
+      <c r="M16">
+        <v>0.19692266116272999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>7.67758071</v>
+      </c>
+      <c r="C17">
+        <v>2.3635674938519001E-2</v>
+      </c>
+      <c r="G17">
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>7.7358897139999998</v>
+      </c>
+      <c r="I17">
+        <v>2.36300157502379E-2</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>6.6681812399999902</v>
+      </c>
+      <c r="M17">
+        <v>0.202254206219911</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>7.8351304079999897</v>
+      </c>
+      <c r="C18">
+        <v>2.36207099954957E-2</v>
+      </c>
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>7.789710328</v>
+      </c>
+      <c r="I18">
+        <v>2.3621782838380199E-2</v>
+      </c>
+      <c r="K18">
+        <v>17</v>
+      </c>
+      <c r="L18">
+        <v>6.3465789599999898</v>
+      </c>
+      <c r="M18">
+        <v>0.19549251969238399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>7.9032242420000003</v>
+      </c>
+      <c r="C19">
+        <v>2.3608125202996301E-2</v>
+      </c>
+      <c r="G19">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>7.73432420199999</v>
+      </c>
+      <c r="I19">
+        <v>2.3630905011029199E-2</v>
+      </c>
+      <c r="K19">
+        <v>18</v>
+      </c>
+      <c r="L19">
+        <v>6.6941064199999998</v>
+      </c>
+      <c r="M19">
+        <v>0.19953212070149001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>8.0147961520000006</v>
+      </c>
+      <c r="C20">
+        <v>2.35860547360035E-2</v>
+      </c>
+      <c r="G20">
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>7.7038543519999996</v>
+      </c>
+      <c r="I20">
+        <v>2.3633705121885399E-2</v>
+      </c>
+      <c r="K20">
+        <v>19</v>
+      </c>
+      <c r="L20">
+        <v>6.9027946800000004</v>
+      </c>
+      <c r="M20">
+        <v>0.20357750874362199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>8.1106760799999993</v>
+      </c>
+      <c r="C21">
+        <v>2.3566766457542101E-2</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>7.7237069680000001</v>
+      </c>
+      <c r="I21">
+        <v>2.36327789001173E-2</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="L21">
+        <v>6.8633185599999997</v>
+      </c>
+      <c r="M21">
+        <v>0.20457930186663301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>10000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>1500</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>1118.73774449999</v>
+      </c>
+      <c r="T31">
+        <v>5.0744873649891904</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>1173.1713883</v>
+      </c>
+      <c r="C32">
+        <v>4.8640315089152697</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1121.12595159999</v>
+      </c>
+      <c r="T32">
+        <v>5.0557357438877704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>1167.6768858999901</v>
+      </c>
+      <c r="C33">
+        <v>4.8893061577955397</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>1132.2439503999999</v>
+      </c>
+      <c r="T33">
+        <v>5.0285307069710603</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>1192.5617689000001</v>
+      </c>
+      <c r="C34">
+        <v>4.7665763753735204</v>
+      </c>
+      <c r="R34">
+        <v>3</v>
+      </c>
+      <c r="S34">
+        <v>1144.58214169999</v>
+      </c>
+      <c r="T34">
+        <v>4.98549233413216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>1201.3945151999999</v>
+      </c>
+      <c r="C35">
+        <v>4.6903443198632502</v>
+      </c>
+      <c r="R35">
+        <v>4</v>
+      </c>
+      <c r="S35">
+        <v>1148.6559431000001</v>
+      </c>
+      <c r="T35">
+        <v>4.9554420860744104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>1201.5473526999999</v>
+      </c>
+      <c r="C36">
+        <v>4.7150197197733297</v>
+      </c>
+      <c r="R36">
+        <v>5</v>
+      </c>
+      <c r="S36">
+        <v>1151.6292277999901</v>
+      </c>
+      <c r="T36">
+        <v>4.9293196932576002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>1211.54486059999</v>
+      </c>
+      <c r="C37">
+        <v>4.6379407739051199</v>
+      </c>
+      <c r="R37">
+        <v>6</v>
+      </c>
+      <c r="S37">
+        <v>1160.9782855000001</v>
+      </c>
+      <c r="T37">
+        <v>4.9256184868217696</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>1207.7114609</v>
+      </c>
+      <c r="C38">
+        <v>4.6676500476096097</v>
+      </c>
+      <c r="R38">
+        <v>7</v>
+      </c>
+      <c r="S38">
+        <v>1163.7738711</v>
+      </c>
+      <c r="T38">
+        <v>4.8952311458320299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>1226.9916456000001</v>
+      </c>
+      <c r="C39">
+        <v>4.5975781973472003</v>
+      </c>
+      <c r="R39">
+        <v>8</v>
+      </c>
+      <c r="S39">
+        <v>1173.1713883</v>
+      </c>
+      <c r="T39">
+        <v>4.8640315089152697</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <v>1225.9456232999901</v>
+      </c>
+      <c r="C40">
+        <v>4.5685409393618297</v>
+      </c>
+      <c r="R40">
+        <v>9</v>
+      </c>
+      <c r="S40">
+        <v>1167.6768858999901</v>
+      </c>
+      <c r="T40">
+        <v>4.8893061577955397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>17</v>
+      </c>
+      <c r="B41">
+        <v>1240.5849143999999</v>
+      </c>
+      <c r="C41">
+        <v>4.48546976227136</v>
+      </c>
+      <c r="R41">
+        <v>10</v>
+      </c>
+      <c r="S41">
+        <v>1192.5617689000001</v>
+      </c>
+      <c r="T41">
+        <v>4.7665763753735204</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18</v>
+      </c>
+      <c r="B42">
+        <v>1235.3133806000001</v>
+      </c>
+      <c r="C42">
+        <v>4.5290597854344803</v>
+      </c>
+      <c r="R42">
+        <v>11</v>
+      </c>
+      <c r="S42">
+        <v>1201.3945151999999</v>
+      </c>
+      <c r="T42">
+        <v>4.6903443198632502</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>19</v>
+      </c>
+      <c r="B43">
+        <v>1246.72590729999</v>
+      </c>
+      <c r="C43">
+        <v>4.4306149110481696</v>
+      </c>
+      <c r="R43">
+        <v>12</v>
+      </c>
+      <c r="S43">
+        <v>1201.5473526999999</v>
+      </c>
+      <c r="T43">
+        <v>4.7150197197733297</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>1257.0787886999999</v>
+      </c>
+      <c r="C44">
+        <v>4.3630310760600404</v>
+      </c>
+      <c r="R44">
+        <v>13</v>
+      </c>
+      <c r="S44">
+        <v>1211.54486059999</v>
+      </c>
+      <c r="T44">
+        <v>4.6379407739051199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>14</v>
+      </c>
+      <c r="S45">
+        <v>1207.7114609</v>
+      </c>
+      <c r="T45">
+        <v>4.6676500476096097</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>15</v>
+      </c>
+      <c r="S46">
+        <v>1226.9916456000001</v>
+      </c>
+      <c r="T46">
+        <v>4.5975781973472003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>16</v>
+      </c>
+      <c r="S47">
+        <v>1225.9456232999901</v>
+      </c>
+      <c r="T47">
+        <v>4.5685409393618297</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>17</v>
+      </c>
+      <c r="S48">
+        <v>1240.5849143999999</v>
+      </c>
+      <c r="T48">
+        <v>4.48546976227136</v>
+      </c>
+    </row>
+    <row r="49" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>18</v>
+      </c>
+      <c r="S49">
+        <v>1235.3133806000001</v>
+      </c>
+      <c r="T49">
+        <v>4.5290597854344803</v>
+      </c>
+    </row>
+    <row r="50" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>19</v>
+      </c>
+      <c r="S50">
+        <v>1246.72590729999</v>
+      </c>
+      <c r="T50">
+        <v>4.4306149110481696</v>
+      </c>
+    </row>
+    <row r="51" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R51">
+        <v>20</v>
+      </c>
+      <c r="S51">
+        <v>1257.0787886999999</v>
+      </c>
+      <c r="T51">
+        <v>4.3630310760600404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="3">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>